<commit_message>
penambahan deskripsi pada projek
</commit_message>
<xml_diff>
--- a/page/excel/REKAP JUNI20251.xlsx
+++ b/page/excel/REKAP JUNI20251.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CPN_ADMIN\Pictures\DATA CHEKPOINT\DATA CHEKPOINT\DATA TAGIHAN\2025\JUNI 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Videos\projek_prtofolio\page\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB81B52F-7654-4EE3-B9E8-3FAA2FCE42A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F95861E-63E1-4BC7-9471-30AF557E18FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A37C67A-AEF1-4F84-859E-F6FAA6AD3406}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{8A37C67A-AEF1-4F84-859E-F6FAA6AD3406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6752,37 +6752,37 @@
     <t>SUTRIS</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>Column8</t>
-  </si>
-  <si>
-    <t>Column9</t>
-  </si>
-  <si>
-    <t>Column10</t>
-  </si>
-  <si>
-    <t>Column11</t>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>tanggal</t>
+  </si>
+  <si>
+    <t>no deliveri</t>
+  </si>
+  <si>
+    <t>tipe muatan</t>
+  </si>
+  <si>
+    <t>nama pt</t>
+  </si>
+  <si>
+    <t>jenis kendaraan</t>
+  </si>
+  <si>
+    <t>no polisi</t>
+  </si>
+  <si>
+    <t>no kontener</t>
+  </si>
+  <si>
+    <t>tujuan</t>
+  </si>
+  <si>
+    <t>nama driver</t>
+  </si>
+  <si>
+    <t>nama admin</t>
   </si>
 </sst>
 </file>
@@ -7755,7 +7755,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column2" xr10:uid="{B8692BE2-E297-4ECD-9476-E426A9184C08}" sourceName="Column2">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column2" xr10:uid="{B8692BE2-E297-4ECD-9476-E426A9184C08}" sourceName="tanggal">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="2"/>
@@ -7765,7 +7765,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column4" xr10:uid="{7C3A70A5-7B60-4942-BAAC-805E824B2434}" sourceName="Column4">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column4" xr10:uid="{7C3A70A5-7B60-4942-BAAC-805E824B2434}" sourceName="tipe muatan">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="4"/>
@@ -7775,7 +7775,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column5" xr10:uid="{6F660973-B170-4EC5-BD94-92921AE4D05E}" sourceName="Column5">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column5" xr10:uid="{6F660973-B170-4EC5-BD94-92921AE4D05E}" sourceName="nama pt">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="5"/>
@@ -7785,7 +7785,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column6" xr10:uid="{BFAAAC10-F4BD-434E-AF77-01AEDB675582}" sourceName="Column6">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Column6" xr10:uid="{BFAAAC10-F4BD-434E-AF77-01AEDB675582}" sourceName="jenis kendaraan">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="6"/>
@@ -7796,10 +7796,10 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Column2" xr10:uid="{90B2926C-D214-46D1-B634-2FFD89EDB6BC}" cache="Slicer_Column2" caption="Column2" columnCount="4" rowHeight="241300"/>
-  <slicer name="Column4" xr10:uid="{15A86A97-82FE-4F83-B66D-23246D64A440}" cache="Slicer_Column4" caption="Column4" rowHeight="241300"/>
-  <slicer name="Column5" xr10:uid="{A106C547-99E8-4B99-91B3-5C16AD5BF88C}" cache="Slicer_Column5" caption="Column5" columnCount="4" rowHeight="241300"/>
-  <slicer name="Column6" xr10:uid="{476057B4-8CEE-4708-BD1C-AD358147AC20}" cache="Slicer_Column6" caption="Column6" rowHeight="241300"/>
+  <slicer name="Column2" xr10:uid="{90B2926C-D214-46D1-B634-2FFD89EDB6BC}" cache="Slicer_Column2" caption="tanggal" columnCount="4" rowHeight="241300"/>
+  <slicer name="Column4" xr10:uid="{15A86A97-82FE-4F83-B66D-23246D64A440}" cache="Slicer_Column4" caption="tipe muatan" rowHeight="241300"/>
+  <slicer name="Column5" xr10:uid="{A106C547-99E8-4B99-91B3-5C16AD5BF88C}" cache="Slicer_Column5" caption="nama pt" columnCount="4" rowHeight="241300"/>
+  <slicer name="Column6" xr10:uid="{476057B4-8CEE-4708-BD1C-AD358147AC20}" cache="Slicer_Column6" caption="jenis kendaraan" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -7807,17 +7807,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF273C02-AED0-4C65-90B1-D68659AC21C4}" name="Table1" displayName="Table1" ref="A17:K1502" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A17:K1502" xr:uid="{AF273C02-AED0-4C65-90B1-D68659AC21C4}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{55B79590-DC2F-4B4D-992B-FE46C1E5399F}" name="Column1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A8B9CACF-7A37-4AAC-A06B-3323961D2CCD}" name="Column2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3D13E001-1FF3-41A1-A540-F499D95DF3ED}" name="Column3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{CD0E24C6-F370-45BE-9064-1261B40030AA}" name="Column4" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{28546300-338D-4519-9CE5-D39E24537059}" name="Column5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{9406F9B6-3AC4-4AF6-98B3-D6230FBE5498}" name="Column6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{8A27EF5A-686E-4AF9-82D8-597CB30DB857}" name="Column7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{339CC161-5476-43CD-B674-94AF970F7DC3}" name="Column8" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{AAAC2222-7628-4EE1-AF40-FA5A4051DC02}" name="Column9" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{2A7D0136-DAA4-4678-B5EF-47157A8C50B8}" name="Column10" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{662C065B-4EAB-4B74-80A0-7BA3D45B44FD}" name="Column11" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{55B79590-DC2F-4B4D-992B-FE46C1E5399F}" name="timestamp" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A8B9CACF-7A37-4AAC-A06B-3323961D2CCD}" name="tanggal" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{3D13E001-1FF3-41A1-A540-F499D95DF3ED}" name="no deliveri" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{CD0E24C6-F370-45BE-9064-1261B40030AA}" name="tipe muatan" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{28546300-338D-4519-9CE5-D39E24537059}" name="nama pt" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{9406F9B6-3AC4-4AF6-98B3-D6230FBE5498}" name="jenis kendaraan" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{8A27EF5A-686E-4AF9-82D8-597CB30DB857}" name="no polisi" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{339CC161-5476-43CD-B674-94AF970F7DC3}" name="no kontener" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{AAAC2222-7628-4EE1-AF40-FA5A4051DC02}" name="tujuan" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{2A7D0136-DAA4-4678-B5EF-47157A8C50B8}" name="nama driver" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{662C065B-4EAB-4B74-80A0-7BA3D45B44FD}" name="nama admin" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8122,8 +8122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034D0457-3CEB-4E3C-93E3-258401B03713}">
   <dimension ref="A16:U1502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1353" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>